<commit_message>
우울 판정 django redis task 연동
</commit_message>
<xml_diff>
--- a/server/nlpsort.xlsx
+++ b/server/nlpsort.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>하</t>
+          <t>죽</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -457,18 +457,18 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>제가</t>
+          <t>요즘</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>NNP</t>
+          <t>NNG</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -478,12 +478,12 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>선생님</t>
+          <t>부모</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>NNP</t>
+          <t>NNG</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -493,12 +493,12 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>귀찮</t>
+          <t>사이</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VA</t>
+          <t>NNG</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -508,12 +508,12 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>모든</t>
+          <t>너무</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>MM</t>
+          <t>MAG</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -523,150 +523,15 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>끝장</t>
+          <t>좋</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>NNG</t>
+          <t>VA</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>내</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>VV</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>문제</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>NNG</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>사람</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>NNG</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>폐</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>NNG</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>끼치</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>VV</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>노력</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>NNG</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>금요일</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>NNP</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>너무</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>MAG</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>바쁘</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>VA</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>